<commit_message>
Phase 4 (December) Update 1 (NT)
</commit_message>
<xml_diff>
--- a/Notes/survey_1.xlsx
+++ b/Notes/survey_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="156">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve">Drawbacks</t>
   </si>
   <si>
+    <t xml:space="preserve">Solution tipe</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chatila &amp; Laumond</t>
   </si>
   <si>
@@ -67,6 +70,9 @@
     <t xml:space="preserve">EKF-SLAM</t>
   </si>
   <si>
+    <t xml:space="preserve">Statistical</t>
+  </si>
+  <si>
     <t xml:space="preserve">Localization of Autonomous Guided Vehicles</t>
   </si>
   <si>
@@ -121,7 +127,7 @@
     <t xml:space="preserve">KLD, Particle Reduction</t>
   </si>
   <si>
-    <t xml:space="preserve">Murangira, Musso, &amp; Dahia, 2016; Zhao, Wang, Qin, &amp; Zhang</t>
+    <t xml:space="preserve">Murangira, Musso, &amp; Dahia</t>
   </si>
   <si>
     <t xml:space="preserve">Rao-Blackwellised Particle Filter</t>
@@ -130,6 +136,9 @@
     <t xml:space="preserve">RBPF, Particle Reduction</t>
   </si>
   <si>
+    <t xml:space="preserve"> Zhao, Wang, Qin, &amp; Zhang</t>
+  </si>
+  <si>
     <t xml:space="preserve">Grisetti, Stachniss, &amp; Burgard</t>
   </si>
   <si>
@@ -196,15 +205,15 @@
     <t xml:space="preserve">Critique of Pro-SLAM</t>
   </si>
   <si>
-    <t xml:space="preserve">2007, 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grisetti et al.; Donoso, Austin, McAree</t>
+    <t xml:space="preserve">Grisetti et al.; </t>
   </si>
   <si>
     <t xml:space="preserve">Iterative Closest Point, Scan Matching</t>
   </si>
   <si>
+    <t xml:space="preserve"> Donoso, Austin, McAree</t>
+  </si>
+  <si>
     <t xml:space="preserve">Newcombe, Lovegrove, and Davison</t>
   </si>
   <si>
@@ -373,7 +382,10 @@
     <t xml:space="preserve">Intelligent robotics and autonomous agents</t>
   </si>
   <si>
-    <t xml:space="preserve">H. Durrant-Whyte and T. Bailey</t>
+    <t xml:space="preserve">G. Borghi and V. Caglioti, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum uncertainty explorations in the self-localization of mobile robots</t>
   </si>
   <si>
     <t xml:space="preserve">G. Grisetti, R. Kummerle, C. Stachniss, and W. Burgard</t>
@@ -472,6 +484,7 @@
         <sz val="10"/>
         <rFont val="Times-Italic"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">exploration–exploitation dilemma</t>
     </r>
@@ -480,6 +493,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.</t>
     </r>
@@ -501,7 +515,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -525,8 +539,26 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -534,11 +566,7 @@
       <sz val="10"/>
       <name val="Times-Italic"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -583,7 +611,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -600,6 +628,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -608,7 +644,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -621,6 +661,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FFC9211E"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -735,16 +835,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A66" activeCellId="0" sqref="A66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C62" activeCellId="0" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="48.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.64"/>
   </cols>
@@ -768,16 +868,19 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1985</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -785,21 +888,21 @@
         <v>1986</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="3" t="n">
         <v>1990</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -807,13 +910,16 @@
         <v>1991</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="E5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -821,13 +927,13 @@
         <v>1995</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -835,24 +941,24 @@
         <v>1997</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="3" t="n">
         <v>2019</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -860,13 +966,13 @@
         <v>2020</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -874,16 +980,16 @@
         <v>2002</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -891,46 +997,46 @@
         <v>2017</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
+        <v>2016</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="n">
         <v>2018</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
-        <v>2007</v>
-      </c>
       <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>2004</v>
+        <v>2007</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>39</v>
@@ -938,27 +1044,27 @@
       <c r="D14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
-        <v>2003</v>
-      </c>
-      <c r="C16" s="1" t="s">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>2004</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E15" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>2007</v>
+        <v>2003</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>45</v>
@@ -971,22 +1077,22 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="1" t="n">
+        <v>2007</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="1" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
-        <v>2018</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>52</v>
@@ -997,24 +1103,27 @@
       <c r="E19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
+        <v>2018</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
         <v>2020</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>59</v>
@@ -1025,150 +1134,144 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>2011</v>
-      </c>
-      <c r="C22" s="1" t="s">
+        <v>2007</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>61</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
-        <v>2020</v>
+        <v>2014</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
-        <v>2010</v>
+        <v>2017</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
-        <v>2011</v>
+        <v>2020</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
-        <v>2019</v>
+        <v>2010</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
-        <v>1992</v>
+        <v>2011</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
-        <v>2012</v>
+        <v>2019</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
-        <v>2008</v>
+        <v>1992</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1176,88 +1279,88 @@
         <v>2012</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
-        <v>2011</v>
+        <v>2008</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
-        <v>2018</v>
+        <v>2012</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="1" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="n">
+        <v>2011</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
-        <v>2013</v>
+        <v>2018</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
-        <v>2013</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1265,211 +1368,223 @@
         <v>2013</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
+        <v>2015</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="n">
+        <v>2013</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="n">
         <v>2018</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
+      <c r="C43" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="n">
         <v>2005</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
-        <v>2006</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
-        <v>2010</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>118</v>
       </c>
+      <c r="D46" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="E46" s="1" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
+      <c r="A47" s="1" t="n">
+        <v>1998</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="n">
+        <v>2006</v>
+      </c>
+      <c r="C48" s="8"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="n">
         <v>2016</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
-        <v>1985</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
-        <v>1988</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="n">
-        <v>1988</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="n">
-        <v>2014</v>
+      <c r="A51" s="1" t="n">
+        <v>1985</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>125</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F51" s="5" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="n">
+      <c r="A52" s="1" t="n">
         <v>1988</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
+      <c r="A53" s="1" t="n">
+        <v>1988</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="n">
+        <v>1988</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="n">
         <v>1985</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="n">
+      <c r="C56" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="n">
         <v>1993</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="n">
+      <c r="C57" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="3" t="n">
         <v>1997</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="n">
+      <c r="C58" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="n">
         <v>1999</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="n">
+      <c r="C59" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="n">
         <v>2020</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C60" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F60" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F57" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="n">
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="n">
         <v>1998</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="n">
-        <v>1998</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="n">
-        <v>2020</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>139</v>
@@ -1477,63 +1592,88 @@
       <c r="D61" s="1" t="s">
         <v>140</v>
       </c>
+      <c r="F61" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="n">
+      <c r="A62" s="1" t="n">
+        <v>1998</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="n">
         <v>1999</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
+      <c r="C65" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="n">
         <v>2012</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="n">
+      <c r="C66" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="n">
         <v>2002</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="n">
+      <c r="C67" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="n">
         <v>1991</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="n">
+      <c r="C68" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="n">
         <v>1999</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>151</v>
+      <c r="C69" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2025 Update #1 NT
</commit_message>
<xml_diff>
--- a/Notes/survey_1.xlsx
+++ b/Notes/survey_1.xlsx
@@ -475,7 +475,7 @@
     <t xml:space="preserve">Coined the term Active SLAM</t>
   </si>
   <si>
-    <t xml:space="preserve">Thurn and Moller</t>
+    <t xml:space="preserve">Thrun and Moller</t>
   </si>
   <si>
     <r>
@@ -515,7 +515,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -549,11 +549,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -611,7 +606,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -632,23 +627,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -837,8 +824,8 @@
   </sheetPr>
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C62" activeCellId="0" sqref="C62"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C69" activeCellId="0" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1010,10 +997,10 @@
       <c r="A12" s="1" t="n">
         <v>2016</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -1027,7 +1014,7 @@
       <c r="C13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>36</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -1136,7 +1123,7 @@
       <c r="A22" s="1" t="n">
         <v>2007</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -1431,10 +1418,10 @@
       <c r="A47" s="1" t="n">
         <v>1998</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="2" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1442,7 +1429,7 @@
       <c r="A48" s="1" t="n">
         <v>2006</v>
       </c>
-      <c r="C48" s="8"/>
+      <c r="C48" s="6"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
@@ -1658,7 +1645,7 @@
       <c r="C68" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D68" s="9" t="s">
+      <c r="D68" s="7" t="s">
         <v>152</v>
       </c>
       <c r="F68" s="2" t="s">

</xml_diff>